<commit_message>
Atualização do repositório de analytics
</commit_message>
<xml_diff>
--- a/Cases/Power BI/case 01/data/Dataset_Vendas.xlsx
+++ b/Cases/Power BI/case 01/data/Dataset_Vendas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://people.ey.com/personal/marco_alencastro_br_ey_com/Documents/Documents/Repos_Git/Analytics/Cases/Power BI/case 01/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_3CE740194F92BCAD8F09588CF136E5CDCD5EFFED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1A5AFAB-DB51-4F91-8886-A33C41F49E45}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_3CE740194F92BCAD8F09588CF136E5CDCD5EFFED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9420AE14-81DE-4796-9B0D-0611AE05DD9E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -866,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A482" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I501"/>
+    <sheetView tabSelected="1" topLeftCell="A398" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13:I411"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -934,7 +934,7 @@
         <v>2200</v>
       </c>
       <c r="I2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -963,7 +963,7 @@
         <v>1600</v>
       </c>
       <c r="I3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -1021,7 +1021,7 @@
         <v>3600</v>
       </c>
       <c r="I5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1050,7 +1050,7 @@
         <v>2000</v>
       </c>
       <c r="I6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -1137,7 +1137,7 @@
         <v>11200</v>
       </c>
       <c r="I9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1195,7 +1195,7 @@
         <v>3500</v>
       </c>
       <c r="I11" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -1224,7 +1224,7 @@
         <v>2000</v>
       </c>
       <c r="I12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -1253,7 +1253,7 @@
         <v>1800</v>
       </c>
       <c r="I13" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -1398,7 +1398,7 @@
         <v>600</v>
       </c>
       <c r="I18" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -1456,7 +1456,7 @@
         <v>2400</v>
       </c>
       <c r="I20" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -1514,7 +1514,7 @@
         <v>14000</v>
       </c>
       <c r="I22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -1543,7 +1543,7 @@
         <v>2000</v>
       </c>
       <c r="I23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -1688,7 +1688,7 @@
         <v>7500</v>
       </c>
       <c r="I28" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
@@ -1717,7 +1717,7 @@
         <v>2800</v>
       </c>
       <c r="I29" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
@@ -1862,7 +1862,7 @@
         <v>2400</v>
       </c>
       <c r="I34" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
@@ -1891,7 +1891,7 @@
         <v>2400</v>
       </c>
       <c r="I35" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
@@ -1949,7 +1949,7 @@
         <v>600</v>
       </c>
       <c r="I37" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
@@ -1978,7 +1978,7 @@
         <v>1000</v>
       </c>
       <c r="I38" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
@@ -2065,7 +2065,7 @@
         <v>1350</v>
       </c>
       <c r="I41" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
@@ -2123,7 +2123,7 @@
         <v>900</v>
       </c>
       <c r="I43" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
@@ -2239,7 +2239,7 @@
         <v>1200</v>
       </c>
       <c r="I47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
@@ -2268,7 +2268,7 @@
         <v>900</v>
       </c>
       <c r="I48" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
@@ -2355,7 +2355,7 @@
         <v>2400</v>
       </c>
       <c r="I51" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
@@ -2442,7 +2442,7 @@
         <v>300</v>
       </c>
       <c r="I54" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
@@ -2471,7 +2471,7 @@
         <v>750</v>
       </c>
       <c r="I55" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
@@ -2500,7 +2500,7 @@
         <v>1800</v>
       </c>
       <c r="I56" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
@@ -2674,7 +2674,7 @@
         <v>500</v>
       </c>
       <c r="I62" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
@@ -2732,7 +2732,7 @@
         <v>7500</v>
       </c>
       <c r="I64" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
@@ -2761,7 +2761,7 @@
         <v>1800</v>
       </c>
       <c r="I65" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
@@ -2848,7 +2848,7 @@
         <v>8400</v>
       </c>
       <c r="I68" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
@@ -2964,7 +2964,7 @@
         <v>1500</v>
       </c>
       <c r="I72" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
@@ -3051,7 +3051,7 @@
         <v>1200</v>
       </c>
       <c r="I75" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
@@ -3167,7 +3167,7 @@
         <v>7500</v>
       </c>
       <c r="I79" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
@@ -3196,7 +3196,7 @@
         <v>10500</v>
       </c>
       <c r="I80" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
@@ -3225,7 +3225,7 @@
         <v>300</v>
       </c>
       <c r="I81" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
@@ -3254,7 +3254,7 @@
         <v>1200</v>
       </c>
       <c r="I82" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
@@ -3283,7 +3283,7 @@
         <v>1600</v>
       </c>
       <c r="I83" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
@@ -3312,7 +3312,7 @@
         <v>2400</v>
       </c>
       <c r="I84" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
@@ -3341,7 +3341,7 @@
         <v>3000</v>
       </c>
       <c r="I85" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
@@ -3370,7 +3370,7 @@
         <v>5600</v>
       </c>
       <c r="I86" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
@@ -3399,7 +3399,7 @@
         <v>6400</v>
       </c>
       <c r="I87" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
@@ -3428,7 +3428,7 @@
         <v>9600</v>
       </c>
       <c r="I88" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
@@ -3457,7 +3457,7 @@
         <v>1200</v>
       </c>
       <c r="I89" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
@@ -3486,7 +3486,7 @@
         <v>17500</v>
       </c>
       <c r="I90" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
@@ -3573,7 +3573,7 @@
         <v>2500</v>
       </c>
       <c r="I93" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
@@ -3631,7 +3631,7 @@
         <v>4800</v>
       </c>
       <c r="I95" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
@@ -3660,7 +3660,7 @@
         <v>4500</v>
       </c>
       <c r="I96" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
@@ -3689,7 +3689,7 @@
         <v>300</v>
       </c>
       <c r="I97" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
@@ -3718,7 +3718,7 @@
         <v>2250</v>
       </c>
       <c r="I98" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
@@ -3834,7 +3834,7 @@
         <v>300</v>
       </c>
       <c r="I102" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
@@ -3863,7 +3863,7 @@
         <v>100</v>
       </c>
       <c r="I103" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.35">
@@ -4008,7 +4008,7 @@
         <v>200</v>
       </c>
       <c r="I108" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
@@ -4066,7 +4066,7 @@
         <v>800</v>
       </c>
       <c r="I110" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.35">
@@ -4182,7 +4182,7 @@
         <v>7500</v>
       </c>
       <c r="I114" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.35">
@@ -4211,7 +4211,7 @@
         <v>2250</v>
       </c>
       <c r="I115" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.35">
@@ -4298,7 +4298,7 @@
         <v>1000</v>
       </c>
       <c r="I118" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.35">
@@ -4356,7 +4356,7 @@
         <v>2400</v>
       </c>
       <c r="I120" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.35">
@@ -4385,7 +4385,7 @@
         <v>6000</v>
       </c>
       <c r="I121" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.35">
@@ -4414,7 +4414,7 @@
         <v>1200</v>
       </c>
       <c r="I122" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.35">
@@ -4472,7 +4472,7 @@
         <v>300</v>
       </c>
       <c r="I124" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.35">
@@ -4617,7 +4617,7 @@
         <v>7500</v>
       </c>
       <c r="I129" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.35">
@@ -4849,7 +4849,7 @@
         <v>6000</v>
       </c>
       <c r="I137" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.35">
@@ -4878,7 +4878,7 @@
         <v>8400</v>
       </c>
       <c r="I138" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.35">
@@ -4907,7 +4907,7 @@
         <v>1600</v>
       </c>
       <c r="I139" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.35">
@@ -5081,7 +5081,7 @@
         <v>1800</v>
       </c>
       <c r="I145" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.35">
@@ -5110,7 +5110,7 @@
         <v>1600</v>
       </c>
       <c r="I146" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.35">
@@ -5197,7 +5197,7 @@
         <v>6000</v>
       </c>
       <c r="I149" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.35">
@@ -5255,7 +5255,7 @@
         <v>2500</v>
       </c>
       <c r="I151" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.35">
@@ -5313,7 +5313,7 @@
         <v>2500</v>
       </c>
       <c r="I153" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.35">
@@ -5342,7 +5342,7 @@
         <v>7500</v>
       </c>
       <c r="I154" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.35">
@@ -5371,7 +5371,7 @@
         <v>1200</v>
       </c>
       <c r="I155" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.35">
@@ -5400,7 +5400,7 @@
         <v>450</v>
       </c>
       <c r="I156" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.35">
@@ -5487,7 +5487,7 @@
         <v>300</v>
       </c>
       <c r="I159" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.35">
@@ -5632,7 +5632,7 @@
         <v>300</v>
       </c>
       <c r="I164" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.35">
@@ -5777,7 +5777,7 @@
         <v>2800</v>
       </c>
       <c r="I169" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.35">
@@ -5835,7 +5835,7 @@
         <v>2500</v>
       </c>
       <c r="I171" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.35">
@@ -5951,7 +5951,7 @@
         <v>3500</v>
       </c>
       <c r="I175" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.35">
@@ -6009,7 +6009,7 @@
         <v>5600</v>
       </c>
       <c r="I177" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.35">
@@ -6067,7 +6067,7 @@
         <v>5600</v>
       </c>
       <c r="I179" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.35">
@@ -6096,7 +6096,7 @@
         <v>1200</v>
       </c>
       <c r="I180" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.35">
@@ -6125,7 +6125,7 @@
         <v>1200</v>
       </c>
       <c r="I181" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.35">
@@ -6212,7 +6212,7 @@
         <v>1000</v>
       </c>
       <c r="I184" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.35">
@@ -6386,7 +6386,7 @@
         <v>4500</v>
       </c>
       <c r="I190" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.35">
@@ -6444,7 +6444,7 @@
         <v>3000</v>
       </c>
       <c r="I192" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.35">
@@ -6502,7 +6502,7 @@
         <v>11200</v>
       </c>
       <c r="I194" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.35">
@@ -6560,7 +6560,7 @@
         <v>250</v>
       </c>
       <c r="I196" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.35">
@@ -6618,7 +6618,7 @@
         <v>2200</v>
       </c>
       <c r="I198" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.35">
@@ -6705,7 +6705,7 @@
         <v>750</v>
       </c>
       <c r="I201" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.35">
@@ -6734,7 +6734,7 @@
         <v>5600</v>
       </c>
       <c r="I202" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.35">
@@ -6821,7 +6821,7 @@
         <v>11200</v>
       </c>
       <c r="I205" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.35">
@@ -6879,7 +6879,7 @@
         <v>10000</v>
       </c>
       <c r="I207" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.35">
@@ -7140,7 +7140,7 @@
         <v>2400</v>
       </c>
       <c r="I216" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.35">
@@ -7198,7 +7198,7 @@
         <v>8400</v>
       </c>
       <c r="I218" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.35">
@@ -7285,7 +7285,7 @@
         <v>300</v>
       </c>
       <c r="I221" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.35">
@@ -7372,7 +7372,7 @@
         <v>11000</v>
       </c>
       <c r="I224" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.35">
@@ -7401,7 +7401,7 @@
         <v>2400</v>
       </c>
       <c r="I225" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.35">
@@ -7430,7 +7430,7 @@
         <v>100</v>
       </c>
       <c r="I226" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.35">
@@ -7488,7 +7488,7 @@
         <v>2800</v>
       </c>
       <c r="I228" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.35">
@@ -7517,7 +7517,7 @@
         <v>900</v>
       </c>
       <c r="I229" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.35">
@@ -7546,7 +7546,7 @@
         <v>1800</v>
       </c>
       <c r="I230" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.35">
@@ -7633,7 +7633,7 @@
         <v>2200</v>
       </c>
       <c r="I233" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.35">
@@ -7662,7 +7662,7 @@
         <v>4800</v>
       </c>
       <c r="I234" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.35">
@@ -7691,7 +7691,7 @@
         <v>600</v>
       </c>
       <c r="I235" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.35">
@@ -7720,7 +7720,7 @@
         <v>7500</v>
       </c>
       <c r="I236" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.35">
@@ -7778,7 +7778,7 @@
         <v>11200</v>
       </c>
       <c r="I238" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.35">
@@ -7807,7 +7807,7 @@
         <v>800</v>
       </c>
       <c r="I239" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.35">
@@ -7865,7 +7865,7 @@
         <v>8400</v>
       </c>
       <c r="I241" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.35">
@@ -7894,7 +7894,7 @@
         <v>16000</v>
       </c>
       <c r="I242" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.35">
@@ -7923,7 +7923,7 @@
         <v>1400</v>
       </c>
       <c r="I243" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.35">
@@ -7952,7 +7952,7 @@
         <v>1500</v>
       </c>
       <c r="I244" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.35">
@@ -7981,7 +7981,7 @@
         <v>2100</v>
       </c>
       <c r="I245" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.35">
@@ -8010,7 +8010,7 @@
         <v>500</v>
       </c>
       <c r="I246" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.35">
@@ -8068,7 +8068,7 @@
         <v>2800</v>
       </c>
       <c r="I248" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.35">
@@ -8097,7 +8097,7 @@
         <v>12800</v>
       </c>
       <c r="I249" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.35">
@@ -8155,7 +8155,7 @@
         <v>150</v>
       </c>
       <c r="I251" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="252" spans="1:9" x14ac:dyDescent="0.35">
@@ -8184,7 +8184,7 @@
         <v>3200</v>
       </c>
       <c r="I252" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="253" spans="1:9" x14ac:dyDescent="0.35">
@@ -8213,7 +8213,7 @@
         <v>2200</v>
       </c>
       <c r="I253" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="254" spans="1:9" x14ac:dyDescent="0.35">
@@ -8271,7 +8271,7 @@
         <v>400</v>
       </c>
       <c r="I255" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.35">
@@ -8387,7 +8387,7 @@
         <v>100</v>
       </c>
       <c r="I259" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="260" spans="1:9" x14ac:dyDescent="0.35">
@@ -8416,7 +8416,7 @@
         <v>1200</v>
       </c>
       <c r="I260" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="261" spans="1:9" x14ac:dyDescent="0.35">
@@ -8474,7 +8474,7 @@
         <v>3200</v>
       </c>
       <c r="I262" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="263" spans="1:9" x14ac:dyDescent="0.35">
@@ -8503,7 +8503,7 @@
         <v>1200</v>
       </c>
       <c r="I263" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="264" spans="1:9" x14ac:dyDescent="0.35">
@@ -8561,7 +8561,7 @@
         <v>2800</v>
       </c>
       <c r="I265" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="266" spans="1:9" x14ac:dyDescent="0.35">
@@ -8735,7 +8735,7 @@
         <v>2800</v>
       </c>
       <c r="I271" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="272" spans="1:9" x14ac:dyDescent="0.35">
@@ -8764,7 +8764,7 @@
         <v>1800</v>
       </c>
       <c r="I272" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="273" spans="1:9" x14ac:dyDescent="0.35">
@@ -8793,7 +8793,7 @@
         <v>3600</v>
       </c>
       <c r="I273" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.35">
@@ -8880,7 +8880,7 @@
         <v>1400</v>
       </c>
       <c r="I276" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.35">
@@ -8909,7 +8909,7 @@
         <v>8800</v>
       </c>
       <c r="I277" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.35">
@@ -8996,7 +8996,7 @@
         <v>1600</v>
       </c>
       <c r="I280" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.35">
@@ -9141,7 +9141,7 @@
         <v>300</v>
       </c>
       <c r="I285" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="286" spans="1:9" x14ac:dyDescent="0.35">
@@ -9199,7 +9199,7 @@
         <v>900</v>
       </c>
       <c r="I287" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="288" spans="1:9" x14ac:dyDescent="0.35">
@@ -9228,7 +9228,7 @@
         <v>600</v>
       </c>
       <c r="I288" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="289" spans="1:9" x14ac:dyDescent="0.35">
@@ -9257,7 +9257,7 @@
         <v>600</v>
       </c>
       <c r="I289" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="290" spans="1:9" x14ac:dyDescent="0.35">
@@ -9286,7 +9286,7 @@
         <v>2800</v>
       </c>
       <c r="I290" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.35">
@@ -9344,7 +9344,7 @@
         <v>3200</v>
       </c>
       <c r="I292" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="293" spans="1:9" x14ac:dyDescent="0.35">
@@ -9373,7 +9373,7 @@
         <v>2700</v>
       </c>
       <c r="I293" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="294" spans="1:9" x14ac:dyDescent="0.35">
@@ -9402,7 +9402,7 @@
         <v>900</v>
       </c>
       <c r="I294" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="295" spans="1:9" x14ac:dyDescent="0.35">
@@ -9460,7 +9460,7 @@
         <v>2400</v>
       </c>
       <c r="I296" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="297" spans="1:9" x14ac:dyDescent="0.35">
@@ -9518,7 +9518,7 @@
         <v>14000</v>
       </c>
       <c r="I298" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="299" spans="1:9" x14ac:dyDescent="0.35">
@@ -9547,7 +9547,7 @@
         <v>2000</v>
       </c>
       <c r="I299" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="300" spans="1:9" x14ac:dyDescent="0.35">
@@ -9779,7 +9779,7 @@
         <v>450</v>
       </c>
       <c r="I307" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="308" spans="1:9" x14ac:dyDescent="0.35">
@@ -9808,7 +9808,7 @@
         <v>1500</v>
       </c>
       <c r="I308" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="309" spans="1:9" x14ac:dyDescent="0.35">
@@ -9866,7 +9866,7 @@
         <v>3500</v>
       </c>
       <c r="I310" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="311" spans="1:9" x14ac:dyDescent="0.35">
@@ -9895,7 +9895,7 @@
         <v>3200</v>
       </c>
       <c r="I311" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="312" spans="1:9" x14ac:dyDescent="0.35">
@@ -9924,7 +9924,7 @@
         <v>14000</v>
       </c>
       <c r="I312" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="313" spans="1:9" x14ac:dyDescent="0.35">
@@ -10011,7 +10011,7 @@
         <v>200</v>
       </c>
       <c r="I315" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="316" spans="1:9" x14ac:dyDescent="0.35">
@@ -10272,7 +10272,7 @@
         <v>900</v>
       </c>
       <c r="I324" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="325" spans="1:9" x14ac:dyDescent="0.35">
@@ -10301,7 +10301,7 @@
         <v>2800</v>
       </c>
       <c r="I325" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="326" spans="1:9" x14ac:dyDescent="0.35">
@@ -10330,7 +10330,7 @@
         <v>900</v>
       </c>
       <c r="I326" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="327" spans="1:9" x14ac:dyDescent="0.35">
@@ -10388,7 +10388,7 @@
         <v>1200</v>
       </c>
       <c r="I328" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="329" spans="1:9" x14ac:dyDescent="0.35">
@@ -10504,7 +10504,7 @@
         <v>8400</v>
       </c>
       <c r="I332" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="333" spans="1:9" x14ac:dyDescent="0.35">
@@ -10533,7 +10533,7 @@
         <v>8800</v>
       </c>
       <c r="I333" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="334" spans="1:9" x14ac:dyDescent="0.35">
@@ -10707,7 +10707,7 @@
         <v>11000</v>
       </c>
       <c r="I339" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="340" spans="1:9" x14ac:dyDescent="0.35">
@@ -10736,7 +10736,7 @@
         <v>3200</v>
       </c>
       <c r="I340" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="341" spans="1:9" x14ac:dyDescent="0.35">
@@ -10765,7 +10765,7 @@
         <v>400</v>
       </c>
       <c r="I341" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="342" spans="1:9" x14ac:dyDescent="0.35">
@@ -10823,7 +10823,7 @@
         <v>1000</v>
       </c>
       <c r="I343" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="344" spans="1:9" x14ac:dyDescent="0.35">
@@ -10852,7 +10852,7 @@
         <v>4500</v>
       </c>
       <c r="I344" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="345" spans="1:9" x14ac:dyDescent="0.35">
@@ -10881,7 +10881,7 @@
         <v>250</v>
       </c>
       <c r="I345" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="346" spans="1:9" x14ac:dyDescent="0.35">
@@ -10939,7 +10939,7 @@
         <v>2500</v>
       </c>
       <c r="I347" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="348" spans="1:9" x14ac:dyDescent="0.35">
@@ -10997,7 +10997,7 @@
         <v>200</v>
       </c>
       <c r="I349" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="350" spans="1:9" x14ac:dyDescent="0.35">
@@ -11026,7 +11026,7 @@
         <v>3500</v>
       </c>
       <c r="I350" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="351" spans="1:9" x14ac:dyDescent="0.35">
@@ -11055,7 +11055,7 @@
         <v>6400</v>
       </c>
       <c r="I351" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="352" spans="1:9" x14ac:dyDescent="0.35">
@@ -11113,7 +11113,7 @@
         <v>1500</v>
       </c>
       <c r="I353" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="354" spans="1:9" x14ac:dyDescent="0.35">
@@ -11200,7 +11200,7 @@
         <v>5600</v>
       </c>
       <c r="I356" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="357" spans="1:9" x14ac:dyDescent="0.35">
@@ -11258,7 +11258,7 @@
         <v>16000</v>
       </c>
       <c r="I358" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="359" spans="1:9" x14ac:dyDescent="0.35">
@@ -11287,7 +11287,7 @@
         <v>12500</v>
       </c>
       <c r="I359" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="360" spans="1:9" x14ac:dyDescent="0.35">
@@ -11316,7 +11316,7 @@
         <v>400</v>
       </c>
       <c r="I360" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="361" spans="1:9" x14ac:dyDescent="0.35">
@@ -11345,7 +11345,7 @@
         <v>6600</v>
       </c>
       <c r="I361" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="362" spans="1:9" x14ac:dyDescent="0.35">
@@ -11461,7 +11461,7 @@
         <v>100</v>
       </c>
       <c r="I365" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="366" spans="1:9" x14ac:dyDescent="0.35">
@@ -11490,7 +11490,7 @@
         <v>800</v>
       </c>
       <c r="I366" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="367" spans="1:9" x14ac:dyDescent="0.35">
@@ -11548,7 +11548,7 @@
         <v>7500</v>
       </c>
       <c r="I368" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="369" spans="1:9" x14ac:dyDescent="0.35">
@@ -11577,7 +11577,7 @@
         <v>600</v>
       </c>
       <c r="I369" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="370" spans="1:9" x14ac:dyDescent="0.35">
@@ -11606,7 +11606,7 @@
         <v>12800</v>
       </c>
       <c r="I370" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="371" spans="1:9" x14ac:dyDescent="0.35">
@@ -11635,7 +11635,7 @@
         <v>2200</v>
       </c>
       <c r="I371" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="372" spans="1:9" x14ac:dyDescent="0.35">
@@ -11664,7 +11664,7 @@
         <v>2800</v>
       </c>
       <c r="I372" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="373" spans="1:9" x14ac:dyDescent="0.35">
@@ -11751,7 +11751,7 @@
         <v>7500</v>
       </c>
       <c r="I375" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="376" spans="1:9" x14ac:dyDescent="0.35">
@@ -11780,7 +11780,7 @@
         <v>12500</v>
       </c>
       <c r="I376" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="377" spans="1:9" x14ac:dyDescent="0.35">
@@ -11809,7 +11809,7 @@
         <v>3000</v>
       </c>
       <c r="I377" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="378" spans="1:9" x14ac:dyDescent="0.35">
@@ -11954,7 +11954,7 @@
         <v>6600</v>
       </c>
       <c r="I382" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="383" spans="1:9" x14ac:dyDescent="0.35">
@@ -11983,7 +11983,7 @@
         <v>1800</v>
       </c>
       <c r="I383" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="384" spans="1:9" x14ac:dyDescent="0.35">
@@ -12041,7 +12041,7 @@
         <v>8800</v>
       </c>
       <c r="I385" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="386" spans="1:9" x14ac:dyDescent="0.35">
@@ -12070,7 +12070,7 @@
         <v>300</v>
       </c>
       <c r="I386" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="387" spans="1:9" x14ac:dyDescent="0.35">
@@ -12099,7 +12099,7 @@
         <v>2400</v>
       </c>
       <c r="I387" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="388" spans="1:9" x14ac:dyDescent="0.35">
@@ -12186,7 +12186,7 @@
         <v>3000</v>
       </c>
       <c r="I390" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="391" spans="1:9" x14ac:dyDescent="0.35">
@@ -12215,7 +12215,7 @@
         <v>14000</v>
       </c>
       <c r="I391" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="392" spans="1:9" x14ac:dyDescent="0.35">
@@ -12244,7 +12244,7 @@
         <v>1200</v>
       </c>
       <c r="I392" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="393" spans="1:9" x14ac:dyDescent="0.35">
@@ -12331,7 +12331,7 @@
         <v>7000</v>
       </c>
       <c r="I395" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="396" spans="1:9" x14ac:dyDescent="0.35">
@@ -12389,7 +12389,7 @@
         <v>600</v>
       </c>
       <c r="I397" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="398" spans="1:9" x14ac:dyDescent="0.35">
@@ -12476,7 +12476,7 @@
         <v>3600</v>
       </c>
       <c r="I400" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="401" spans="1:9" x14ac:dyDescent="0.35">
@@ -12534,7 +12534,7 @@
         <v>3500</v>
       </c>
       <c r="I402" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="403" spans="1:9" x14ac:dyDescent="0.35">
@@ -12563,7 +12563,7 @@
         <v>400</v>
       </c>
       <c r="I403" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="404" spans="1:9" x14ac:dyDescent="0.35">
@@ -12592,7 +12592,7 @@
         <v>7500</v>
       </c>
       <c r="I404" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="405" spans="1:9" x14ac:dyDescent="0.35">
@@ -12621,7 +12621,7 @@
         <v>2100</v>
       </c>
       <c r="I405" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="406" spans="1:9" x14ac:dyDescent="0.35">
@@ -12650,7 +12650,7 @@
         <v>7500</v>
       </c>
       <c r="I406" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="407" spans="1:9" x14ac:dyDescent="0.35">
@@ -12679,7 +12679,7 @@
         <v>450</v>
       </c>
       <c r="I407" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="408" spans="1:9" x14ac:dyDescent="0.35">
@@ -12737,7 +12737,7 @@
         <v>3500</v>
       </c>
       <c r="I409" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="410" spans="1:9" x14ac:dyDescent="0.35">
@@ -14970,7 +14970,7 @@
         <v>2700</v>
       </c>
       <c r="I486" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="487" spans="1:9" x14ac:dyDescent="0.35">
@@ -14999,7 +14999,7 @@
         <v>1500</v>
       </c>
       <c r="I487" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="488" spans="1:9" x14ac:dyDescent="0.35">
@@ -15028,7 +15028,7 @@
         <v>2800</v>
       </c>
       <c r="I488" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="489" spans="1:9" x14ac:dyDescent="0.35">
@@ -15115,7 +15115,7 @@
         <v>750</v>
       </c>
       <c r="I491" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="492" spans="1:9" x14ac:dyDescent="0.35">
@@ -15260,7 +15260,7 @@
         <v>7500</v>
       </c>
       <c r="I496" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="497" spans="1:9" x14ac:dyDescent="0.35">
@@ -15376,7 +15376,7 @@
         <v>9600</v>
       </c>
       <c r="I500" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="501" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>